<commit_message>
Avance de revisión bibliográfica
</commit_message>
<xml_diff>
--- a/Material de referencia/Bibliografía/Guía de lectura.xlsx
+++ b/Material de referencia/Bibliografía/Guía de lectura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22524"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar\OneDrive\GitHub\Tesis\Material de referencia\Bibliografía\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3497\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="8_{A04BDD55-48E2-431F-B48B-0FFDEEC3103B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7686952B-CCC1-41A3-8E81-EBA8C607C243}"/>
+  <xr:revisionPtr revIDLastSave="392" documentId="8_{A04BDD55-48E2-431F-B48B-0FFDEEC3103B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7F8CE85-687E-4091-863E-0DE738714449}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{BFE77630-5682-4481-A2C8-A32604FFFC82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{BFE77630-5682-4481-A2C8-A32604FFFC82}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7DEE412F-9890-4DB0-83FE-BF1438DFBF8A}</author>
+    <author>tc={E049BA1F-89ED-44E8-A7F0-25FC7D19D358}</author>
+    <author>tc={282FEB1F-440F-4C68-829C-7CDA39B2C91E}</author>
+  </authors>
+  <commentList>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{7DEE412F-9890-4DB0-83FE-BF1438DFBF8A}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Link de descarga</t>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{E049BA1F-89ED-44E8-A7F0-25FC7D19D358}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Es descartable porque lo que sirve está mejor explicado en el documento 2.
+Las lecturas "04.1-Box-Jenkins Methodology" y "04.2-Box-Jenkins ARIMA forecasting" pueden servir de apoyo para el documento 2.</t>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="2" shapeId="0" xr:uid="{282FEB1F-440F-4C68-829C-7CDA39B2C91E}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Link de descarga gratuita</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="122">
   <si>
     <t>Nombre</t>
   </si>
@@ -394,13 +431,19 @@
   </si>
   <si>
     <t>Para usar las referencias que tiene</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/pdf/10.1177/0256090919880107</t>
+  </si>
+  <si>
+    <t>https://pdfs.semanticscholar.org/7cd4/e19b3eeecf086574969a2cc9d5a4b987275b.pdf?_ga=2.58021998.577057181.1581969273-1619670940.1570123960</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +458,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="7">
@@ -468,13 +516,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,21 +537,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -515,12 +547,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,6 +560,42 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -550,6 +612,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="César Gamboa" id="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" userId="4c0abcc15bdc5c59" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,134 +915,149 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F12" dT="2020-02-17T19:57:08.35" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{7DEE412F-9890-4DB0-83FE-BF1438DFBF8A}">
+    <text>Link de descarga</text>
+  </threadedComment>
+  <threadedComment ref="A13" dT="2020-02-17T19:28:37.40" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{E049BA1F-89ED-44E8-A7F0-25FC7D19D358}">
+    <text>Es descartable porque lo que sirve está mejor explicado en el documento 2.
+Las lecturas "04.1-Box-Jenkins Methodology" y "04.2-Box-Jenkins ARIMA forecasting" pueden servir de apoyo para el documento 2.</text>
+  </threadedComment>
+  <threadedComment ref="F15" dT="2020-02-17T19:52:37.76" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{282FEB1F-440F-4C68-829C-7CDA39B2C91E}">
+    <text>Link de descarga gratuita</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D9E628-5B5B-4B89-A052-7CB3517C8F2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D9E628-5B5B-4B89-A052-7CB3517C8F2F}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.26953125" customWidth="1"/>
-    <col min="4" max="4" width="45.36328125" customWidth="1"/>
-    <col min="5" max="5" width="63.453125" customWidth="1"/>
-    <col min="6" max="6" width="52.453125" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
+    <row r="7" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="24">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>20</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
       <c r="C11" t="s">
@@ -983,75 +1066,78 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+    <row r="12" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="21">
         <v>3</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
         <v>4</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="27">
         <v>4</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="1" t="s">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>9</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>5</v>
       </c>
       <c r="C15" t="s">
@@ -1060,38 +1146,41 @@
       <c r="D15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25">
+    <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
         <v>2</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="17">
         <v>6</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>6</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>7</v>
       </c>
       <c r="C17" t="s">
@@ -1100,21 +1189,21 @@
       <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>7</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>8</v>
       </c>
       <c r="C18" t="s">
@@ -1123,38 +1212,38 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22">
+    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
         <v>1</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="14">
         <v>9</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>15</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>10</v>
       </c>
       <c r="C20" t="s">
@@ -1163,18 +1252,18 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="7">
+      <c r="G20" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>11</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>11</v>
       </c>
       <c r="C21" t="s">
@@ -1183,54 +1272,54 @@
       <c r="D21" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="9">
+      <c r="G21" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
         <v>24</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="24">
         <v>12</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="G22" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+      <c r="G23" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>25</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>13</v>
       </c>
       <c r="C24" t="s">
@@ -1239,21 +1328,21 @@
       <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
+      <c r="G24" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>26</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>14</v>
       </c>
       <c r="C25" t="s">
@@ -1262,21 +1351,21 @@
       <c r="D25" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="7">
+      <c r="G25" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>16</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>15</v>
       </c>
       <c r="C26" t="s">
@@ -1285,18 +1374,18 @@
       <c r="D26" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
+      <c r="G26" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>17</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>16</v>
       </c>
       <c r="C27" t="s">
@@ -1305,18 +1394,18 @@
       <c r="D27" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="7">
+      <c r="G27" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <v>23</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>17</v>
       </c>
       <c r="C28" t="s">
@@ -1325,18 +1414,18 @@
       <c r="D28" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
+      <c r="G28" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>27</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>18</v>
       </c>
       <c r="C29" t="s">
@@ -1345,21 +1434,21 @@
       <c r="D29" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="7">
+      <c r="G29" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>31</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>19</v>
       </c>
       <c r="C30" t="s">
@@ -1368,41 +1457,41 @@
       <c r="D30" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20">
+      <c r="G30" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
         <v>3</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="19">
         <v>20</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="7">
+      <c r="G31" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>29</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>21</v>
       </c>
       <c r="C32" t="s">
@@ -1411,21 +1500,21 @@
       <c r="D32" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="7">
+      <c r="G32" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>14</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>22</v>
       </c>
       <c r="C33" t="s">
@@ -1434,21 +1523,21 @@
       <c r="D33" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>78</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="7">
+      <c r="G33" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>28</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>23</v>
       </c>
       <c r="C34" t="s">
@@ -1457,18 +1546,18 @@
       <c r="D34" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="7">
+      <c r="G34" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
         <v>21</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>24</v>
       </c>
       <c r="C35" t="s">
@@ -1477,21 +1566,21 @@
       <c r="D35" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>83</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="7">
+      <c r="G35" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>32</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>25</v>
       </c>
       <c r="C36" t="s">
@@ -1500,21 +1589,21 @@
       <c r="D36" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="7" t="s">
         <v>86</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="7">
+      <c r="G36" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>12</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>26</v>
       </c>
       <c r="C37" t="s">
@@ -1523,21 +1612,21 @@
       <c r="D37" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>90</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="7">
+      <c r="G37" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
         <v>8</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>27</v>
       </c>
       <c r="C38" t="s">
@@ -1546,21 +1635,21 @@
       <c r="D38" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="7">
+      <c r="G38" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
         <v>30</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>28</v>
       </c>
       <c r="C39" t="s">
@@ -1569,21 +1658,21 @@
       <c r="D39" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="7">
+      <c r="G39" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
         <v>18</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>29</v>
       </c>
       <c r="C40" t="s">
@@ -1592,18 +1681,18 @@
       <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="7">
+      <c r="G40" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>10</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="4">
         <v>30</v>
       </c>
       <c r="C41" t="s">
@@ -1612,18 +1701,18 @@
       <c r="D41" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="7">
+      <c r="G41" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
         <v>13</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>31</v>
       </c>
       <c r="C42" t="s">
@@ -1632,21 +1721,21 @@
       <c r="D42" t="s">
         <v>104</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>105</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="7">
+      <c r="G42" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
         <v>22</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>32</v>
       </c>
       <c r="C43" t="s">
@@ -1655,21 +1744,23 @@
       <c r="D43" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>109</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B44" s="5"/>
+      <c r="G43" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A22:A23"/>
@@ -1685,8 +1776,6 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{822BD789-2E43-42D7-8964-C3A5740768D4}"/>
@@ -1744,9 +1833,12 @@
     <hyperlink ref="F42" r:id="rId53" xr:uid="{F17B67E0-8657-4EF6-8FFC-E5A52A0A74A3}"/>
     <hyperlink ref="E43" r:id="rId54" xr:uid="{1478903D-7E95-4CCA-89D1-CD3F34A457FB}"/>
     <hyperlink ref="F43" r:id="rId55" xr:uid="{8AACD802-C59D-4581-AB2E-188EEEF84EB8}"/>
+    <hyperlink ref="F15" r:id="rId56" xr:uid="{0C13EA24-1FCB-4864-8575-6235B5EC8B6A}"/>
+    <hyperlink ref="F12" r:id="rId57" xr:uid="{DC7110F3-05E6-48B3-B199-5A881DE7351E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
+  <legacyDrawing r:id="rId59"/>
 </worksheet>
 </file>
 
@@ -1758,13 +1850,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1775,355 +1867,355 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="8">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="8">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="14" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="8">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="8">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="8">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="8">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="8">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="8">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+    <row r="23" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="8">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="8">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="8">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="14" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:3" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="8">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
+    <row r="33" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="8">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Código para cronograma tentativo
</commit_message>
<xml_diff>
--- a/Material de referencia/Bibliografía/Guía de lectura.xlsx
+++ b/Material de referencia/Bibliografía/Guía de lectura.xlsx
@@ -1,96 +1,124 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar.gamboa\Documents\Github\Tesis\Material de referencia\Bibliografía\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\GitHub\Tesis\Material de referencia\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="36" documentId="114_{31B711B0-9703-4500-A5BE-1C9B89916F50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E193CC8-F76A-47FA-8100-D141B9F75B00}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={7DEE412F-9890-4DB0-83FE-BF1438DFBF8A}</author>
     <author>tc={E049BA1F-89ED-44E8-A7F0-25FC7D19D358}</author>
     <author>tc={282FEB1F-440F-4C68-829C-7CDA39B2C91E}</author>
+    <author>tc={FE7F24B7-F545-42DC-99A6-B0576309AF5C}</author>
+    <author>tc={F6EC0168-B4E3-4E67-935B-C395D318556F}</author>
+    <author>tc={F00D790E-8BDA-4791-88B0-43F2A6D94E27}</author>
+    <author>tc={4F68D8B3-B9B1-4C07-B123-78FFDB930113}</author>
+    <author>tc={05D0CF0D-7D8F-4DF9-AAB9-33FB2A729B26}</author>
+    <author>tc={6D8A7E0D-840B-4B63-9EB6-B348B45DE0C3}</author>
+    <author>tc={C0047460-3AB5-4AD1-8D31-F291FD47E8E9}</author>
   </authors>
   <commentList>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Link de descarga</t>
-        </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1" shapeId="0">
+    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Es descartable porque lo que sirve está mejor explicado en el documento 2.
 Las lecturas "04.1-Box-Jenkins Methodology" y "04.2-Box-Jenkins ARIMA forecasting" pueden servir de apoyo para el documento 2.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="2" shapeId="0">
+    <comment ref="F15" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Comentario encadenado]
+        <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Link de descarga gratuita</t>
-        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="3" shapeId="0" xr:uid="{FE7F24B7-F545-42DC-99A6-B0576309AF5C}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Sirve a modo de resumen de todo lo referente a los modelos ARIMA.</t>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="4" shapeId="0" xr:uid="{F6EC0168-B4E3-4E67-935B-C395D318556F}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Es solo un caso de estudio con criptomonedas.</t>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="5" shapeId="0" xr:uid="{F00D790E-8BDA-4791-88B0-43F2A6D94E27}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Menciona varias alternativas de métodos automáticos.</t>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="6" shapeId="0" xr:uid="{4F68D8B3-B9B1-4C07-B123-78FFDB930113}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Estaba repetido, ya lo leí en el 19.</t>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="7" shapeId="0" xr:uid="{05D0CF0D-7D8F-4DF9-AAB9-33FB2A729B26}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Se sale de los límites de los modelos lineales y trabaja con Análisis Espectral.</t>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="8" shapeId="0" xr:uid="{6D8A7E0D-840B-4B63-9EB6-B348B45DE0C3}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Otra alternativa para métodos automáticos.</t>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="9" shapeId="0" xr:uid="{C0047460-3AB5-4AD1-8D31-F291FD47E8E9}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Menciona algunas ventajas de unas medidas sobre otras.</t>
       </text>
     </comment>
   </commentList>
@@ -476,8 +504,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +520,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -545,26 +579,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -595,26 +616,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -625,7 +629,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -959,16 +984,37 @@
   <threadedComment ref="F15" dT="2020-02-17T19:52:37.76" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{282FEB1F-440F-4C68-829C-7CDA39B2C91E}">
     <text>Link de descarga gratuita</text>
   </threadedComment>
+  <threadedComment ref="A17" dT="2020-03-04T17:04:28.97" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{FE7F24B7-F545-42DC-99A6-B0576309AF5C}">
+    <text>Sirve a modo de resumen de todo lo referente a los modelos ARIMA.</text>
+  </threadedComment>
+  <threadedComment ref="A18" dT="2020-03-04T17:05:45.14" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{F6EC0168-B4E3-4E67-935B-C395D318556F}">
+    <text>Es solo un caso de estudio con criptomonedas.</text>
+  </threadedComment>
+  <threadedComment ref="A20" dT="2020-03-04T18:15:03.25" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{F00D790E-8BDA-4791-88B0-43F2A6D94E27}">
+    <text>Menciona varias alternativas de métodos automáticos.</text>
+  </threadedComment>
+  <threadedComment ref="A35" dT="2020-03-04T18:21:43.21" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{4F68D8B3-B9B1-4C07-B123-78FFDB930113}">
+    <text>Estaba repetido, ya lo leí en el 19.</text>
+  </threadedComment>
+  <threadedComment ref="A38" dT="2020-03-04T17:17:58.18" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{05D0CF0D-7D8F-4DF9-AAB9-33FB2A729B26}">
+    <text>Se sale de los límites de los modelos lineales y trabaja con Análisis Espectral.</text>
+  </threadedComment>
+  <threadedComment ref="A40" dT="2020-03-04T18:15:18.67" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{6D8A7E0D-840B-4B63-9EB6-B348B45DE0C3}">
+    <text>Otra alternativa para métodos automáticos.</text>
+  </threadedComment>
+  <threadedComment ref="A42" dT="2020-03-04T18:09:44.63" personId="{47302F5D-DC63-433A-BB8A-05B7D442D9E7}" id="{C0047460-3AB5-4AD1-8D31-F291FD47E8E9}">
+    <text>Menciona algunas ventajas de unas medidas sobre otras.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,821 +1028,827 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="11" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>19</v>
       </c>
       <c r="B7" s="26">
         <v>1</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="29" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="1" t="s">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="22" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="1" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="26"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="1" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
         <v>20</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="23">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
         <v>5</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="14">
         <v>3</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>4</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="17">
         <v>4</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="24" t="s">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
         <v>9</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="23">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+    <row r="16" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>2</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="12">
         <v>6</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
         <v>6</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="14">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
         <v>7</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="23">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
         <v>1</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="9">
         <v>9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="14">
         <v>10</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
         <v>11</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="14">
         <v>11</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26">
         <v>24</v>
       </c>
       <c r="B22" s="26">
         <v>12</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="26"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="1" t="s">
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
         <v>25</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="14">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
         <v>26</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="14">
         <v>14</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
         <v>16</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="14">
         <v>15</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
         <v>17</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="14">
         <v>16</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
         <v>23</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="14">
         <v>17</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+    <row r="29" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="23">
         <v>18</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
         <v>31</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="14">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
         <v>3</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="14">
         <v>20</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+    <row r="32" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
         <v>29</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="23">
         <v>21</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
         <v>14</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="23">
         <v>22</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+    <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
         <v>28</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="14">
         <v>23</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+    <row r="35" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
         <v>21</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="23">
         <v>24</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+    <row r="36" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23">
         <v>32</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="23">
         <v>25</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+    <row r="37" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
         <v>12</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="14">
         <v>26</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23">
         <v>8</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="23">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+    <row r="39" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
         <v>30</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="23">
         <v>28</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
         <v>18</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="14">
         <v>29</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+    <row r="41" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
         <v>10</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="14">
         <v>30</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
+    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
         <v>13</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="14">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
+    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
         <v>22</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="14">
         <v>32</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+      <c r="B44" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
@@ -1808,73 +1860,67 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="F7" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F10" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6" display="https://stats.stackexchange.com/questions/14099/using-k-fold-cross-validation-for-time-series-model-selection"/>
-    <hyperlink ref="E11" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
-    <hyperlink ref="E13" r:id="rId11"/>
-    <hyperlink ref="E15" r:id="rId12"/>
-    <hyperlink ref="E16" r:id="rId13"/>
-    <hyperlink ref="E17" r:id="rId14"/>
-    <hyperlink ref="E18" r:id="rId15"/>
-    <hyperlink ref="E19" r:id="rId16"/>
-    <hyperlink ref="F17" r:id="rId17"/>
-    <hyperlink ref="E20" r:id="rId18"/>
-    <hyperlink ref="E21" r:id="rId19"/>
-    <hyperlink ref="E22" r:id="rId20"/>
-    <hyperlink ref="F22" r:id="rId21"/>
-    <hyperlink ref="F23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="F24" r:id="rId24"/>
-    <hyperlink ref="F25" r:id="rId25"/>
-    <hyperlink ref="E25" r:id="rId26"/>
-    <hyperlink ref="E26" r:id="rId27"/>
-    <hyperlink ref="E27" r:id="rId28"/>
-    <hyperlink ref="E28" r:id="rId29"/>
-    <hyperlink ref="E29" r:id="rId30"/>
-    <hyperlink ref="F29" r:id="rId31"/>
-    <hyperlink ref="F30" r:id="rId32"/>
-    <hyperlink ref="E30" r:id="rId33"/>
-    <hyperlink ref="E31" r:id="rId34"/>
-    <hyperlink ref="E32" r:id="rId35"/>
-    <hyperlink ref="F32" r:id="rId36"/>
-    <hyperlink ref="E33" r:id="rId37"/>
-    <hyperlink ref="F33" r:id="rId38"/>
-    <hyperlink ref="E34" r:id="rId39"/>
-    <hyperlink ref="E35" r:id="rId40"/>
-    <hyperlink ref="F35" r:id="rId41"/>
-    <hyperlink ref="E36" r:id="rId42"/>
-    <hyperlink ref="F36" r:id="rId43"/>
-    <hyperlink ref="E37" r:id="rId44"/>
-    <hyperlink ref="F37" r:id="rId45"/>
-    <hyperlink ref="E38" r:id="rId46"/>
-    <hyperlink ref="F38" r:id="rId47"/>
-    <hyperlink ref="E39" r:id="rId48"/>
-    <hyperlink ref="F39" r:id="rId49"/>
-    <hyperlink ref="E40" r:id="rId50"/>
-    <hyperlink ref="E41" r:id="rId51"/>
-    <hyperlink ref="E42" r:id="rId52"/>
-    <hyperlink ref="F42" r:id="rId53"/>
-    <hyperlink ref="E43" r:id="rId54"/>
-    <hyperlink ref="F43" r:id="rId55"/>
-    <hyperlink ref="F15" r:id="rId56"/>
-    <hyperlink ref="F12" r:id="rId57"/>
-    <hyperlink ref="F21" r:id="rId58"/>
-    <hyperlink ref="F40" r:id="rId59"/>
+    <hyperlink ref="E7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F11" r:id="rId6" display="https://stats.stackexchange.com/questions/14099/using-k-fold-cross-validation-for-time-series-model-selection" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F17" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F25" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E26" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E27" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E28" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E29" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F29" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F30" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E30" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E31" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E32" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F32" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E33" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F33" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E34" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E35" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F35" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E36" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F36" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E37" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F37" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E38" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F38" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E39" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F39" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E40" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E41" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E42" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F42" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E43" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F43" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F15" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F12" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F21" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F40" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId60"/>
@@ -1883,7 +1929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1907,360 +1953,360 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:3" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="3">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B38">
     <sortCondition ref="B2:B38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>